<commit_message>
Plot but it's random, still trying the add up demand to zero
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Desktop\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638CD4E0-8BD4-4F54-B621-D37D20130D83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A4C1FD-5DAD-4F0B-8F6A-252E4CB00F56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{BB2F6137-FFDB-4445-AF15-5390304252B2}"/>
   </bookViews>
@@ -40324,7 +40324,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -40341,8 +40341,8 @@
       <c r="A2" t="s">
         <v>65</v>
       </c>
-      <c r="B2">
-        <v>-39.200000000000003</v>
+      <c r="B2" s="8">
+        <v>-39.299999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40350,10 +40350,12 @@
         <v>29</v>
       </c>
       <c r="B3" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8">
         <v>0.71001317696823862</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="7"/>
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40361,10 +40363,13 @@
         <v>30</v>
       </c>
       <c r="B4" s="8">
+        <f t="shared" ref="B4:B34" si="0">ROUND(E4,1)</f>
+        <v>0.9</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8">
         <v>0.85983750298624806</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40372,10 +40377,13 @@
         <v>31</v>
       </c>
       <c r="B5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8">
         <v>0.29582423162100185</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="7"/>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40383,10 +40391,13 @@
         <v>32</v>
       </c>
       <c r="B6" s="8">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8">
         <v>1.6613043664642653</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="7"/>
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40394,10 +40405,13 @@
         <v>33</v>
       </c>
       <c r="B7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8">
         <v>0.88472561777458414</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="7"/>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40405,10 +40419,13 @@
         <v>34</v>
       </c>
       <c r="B8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8">
         <v>0.54997100630889695</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="7"/>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40416,10 +40433,13 @@
         <v>35</v>
       </c>
       <c r="B9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8">
         <v>0.91673310218230786</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="7"/>
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40427,10 +40447,13 @@
         <v>36</v>
       </c>
       <c r="B10" s="8">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8">
         <v>0.55194049675388024</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="7"/>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40438,10 +40461,13 @@
         <v>37</v>
       </c>
       <c r="B11" s="8">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8">
         <v>0.48661253430844403</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7"/>
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40449,10 +40475,13 @@
         <v>38</v>
       </c>
       <c r="B12" s="8">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8">
         <v>0.82711772547003137</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7"/>
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40460,10 +40489,13 @@
         <v>39</v>
       </c>
       <c r="B13" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8">
         <v>1.3694042762934697</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="7"/>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40471,10 +40503,13 @@
         <v>40</v>
       </c>
       <c r="B14" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8">
         <v>1.3035320031976267</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7"/>
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40482,10 +40517,13 @@
         <v>41</v>
       </c>
       <c r="B15" s="8">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8">
         <v>1.0829437311611987</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="7"/>
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40493,10 +40531,13 @@
         <v>42</v>
       </c>
       <c r="B16" s="8">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8">
         <v>0.44587827216650028</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="7"/>
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40504,10 +40545,13 @@
         <v>43</v>
       </c>
       <c r="B17" s="8">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8">
         <v>0.79775225491722634</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="7"/>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40515,10 +40559,13 @@
         <v>44</v>
       </c>
       <c r="B18" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8">
         <v>0.96125735723902472</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="7"/>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40526,10 +40573,13 @@
         <v>45</v>
       </c>
       <c r="B19" s="8">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8">
         <v>1.7197741334300947</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="7"/>
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40537,10 +40587,13 @@
         <v>46</v>
       </c>
       <c r="B20" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8">
         <v>1.4854391979773423</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7"/>
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40548,10 +40601,13 @@
         <v>47</v>
       </c>
       <c r="B21" s="8">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8">
         <v>1.0954676247412771</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="7"/>
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40559,10 +40615,13 @@
         <v>48</v>
       </c>
       <c r="B22" s="8">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8">
         <v>1.0805361804544924</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="7"/>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40570,10 +40629,13 @@
         <v>49</v>
       </c>
       <c r="B23" s="8">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8">
         <v>2.1045335018447622</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="7"/>
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40581,10 +40643,13 @@
         <v>50</v>
       </c>
       <c r="B24" s="8">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8">
         <v>3.1337893271084818</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="7"/>
       <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40592,10 +40657,13 @@
         <v>51</v>
       </c>
       <c r="B25" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8">
         <v>1.4196571486752416</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="7"/>
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40603,9 +40671,12 @@
         <v>52</v>
       </c>
       <c r="B26" s="8">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="E26" s="8">
         <v>1.7083685400303503</v>
       </c>
-      <c r="C26" s="8"/>
       <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40613,9 +40684,12 @@
         <v>53</v>
       </c>
       <c r="B27" s="8">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="E27" s="8">
         <v>1.1745648065514733</v>
       </c>
-      <c r="C27" s="8"/>
       <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40623,9 +40697,12 @@
         <v>54</v>
       </c>
       <c r="B28" s="8">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E28" s="8">
         <v>1.0875837271854403</v>
       </c>
-      <c r="C28" s="8"/>
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40633,9 +40710,12 @@
         <v>55</v>
       </c>
       <c r="B29" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E29" s="8">
         <v>1.4746461766509018</v>
       </c>
-      <c r="C29" s="8"/>
       <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40643,9 +40723,12 @@
         <v>56</v>
       </c>
       <c r="B30" s="8">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="E30" s="8">
         <v>0.78701502988428473</v>
       </c>
-      <c r="C30" s="8"/>
       <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40653,9 +40736,12 @@
         <v>57</v>
       </c>
       <c r="B31" s="8">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="E31" s="8">
         <v>0.33454507857627203</v>
       </c>
-      <c r="C31" s="8"/>
       <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40663,9 +40749,12 @@
         <v>58</v>
       </c>
       <c r="B32" s="8">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="E32" s="8">
         <v>0.70367911050096443</v>
       </c>
-      <c r="C32" s="8"/>
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40673,9 +40762,12 @@
         <v>59</v>
       </c>
       <c r="B33" s="8">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="E33" s="8">
         <v>1.1654320217454122</v>
       </c>
-      <c r="C33" s="8"/>
       <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40683,9 +40775,12 @@
         <v>60</v>
       </c>
       <c r="B34" s="8">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="E34" s="8">
         <v>0.68959588859087695</v>
       </c>
-      <c r="C34" s="8"/>
       <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40693,9 +40788,12 @@
         <v>61</v>
       </c>
       <c r="B35" s="8">
+        <f t="shared" ref="B35:B58" si="1">ROUND(E35,1)</f>
+        <v>3.2</v>
+      </c>
+      <c r="E35" s="8">
         <v>3.2200397124607183</v>
       </c>
-      <c r="C35" s="8"/>
       <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40703,9 +40801,12 @@
         <v>62</v>
       </c>
       <c r="B36" s="8">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E36" s="8">
         <v>1.1104851377786713</v>
       </c>
-      <c r="C36" s="8"/>
       <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -40713,6 +40814,10 @@
         <v>7</v>
       </c>
       <c r="B37" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E37" s="8">
         <v>0</v>
       </c>
     </row>
@@ -40721,6 +40826,10 @@
         <v>8</v>
       </c>
       <c r="B38" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="8">
         <v>0</v>
       </c>
     </row>
@@ -40729,6 +40838,10 @@
         <v>9</v>
       </c>
       <c r="B39" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="8">
         <v>0</v>
       </c>
     </row>
@@ -40737,6 +40850,10 @@
         <v>10</v>
       </c>
       <c r="B40" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E40" s="8">
         <v>0</v>
       </c>
     </row>
@@ -40745,6 +40862,10 @@
         <v>11</v>
       </c>
       <c r="B41" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="8">
         <v>0</v>
       </c>
     </row>
@@ -40753,6 +40874,10 @@
         <v>12</v>
       </c>
       <c r="B42" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="8">
         <v>0</v>
       </c>
     </row>
@@ -40761,6 +40886,10 @@
         <v>13</v>
       </c>
       <c r="B43" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="8">
         <v>0</v>
       </c>
     </row>
@@ -40769,6 +40898,10 @@
         <v>14</v>
       </c>
       <c r="B44" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="8">
         <v>0</v>
       </c>
     </row>
@@ -40777,6 +40910,10 @@
         <v>15</v>
       </c>
       <c r="B45" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="8">
         <v>0</v>
       </c>
     </row>
@@ -40785,6 +40922,10 @@
         <v>16</v>
       </c>
       <c r="B46" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="8">
         <v>0</v>
       </c>
     </row>
@@ -40793,6 +40934,10 @@
         <v>17</v>
       </c>
       <c r="B47" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="8">
         <v>0</v>
       </c>
     </row>
@@ -40801,86 +40946,130 @@
         <v>18</v>
       </c>
       <c r="B48" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="E48" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="E49" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>20</v>
       </c>
       <c r="B50" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="E50" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>21</v>
       </c>
       <c r="B51" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="E51" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>22</v>
       </c>
       <c r="B52" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="E52" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>23</v>
       </c>
       <c r="B53" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="E53" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>24</v>
       </c>
       <c r="B54" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="E54" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>25</v>
       </c>
       <c r="B55" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="E55" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>26</v>
       </c>
       <c r="B56" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="E56" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>27</v>
       </c>
       <c r="B57" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="E57" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>28</v>
       </c>
       <c r="B58" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E58" s="8">
         <v>0</v>
       </c>
     </row>

</xml_diff>